<commit_message>
finished the functionality for the report and creted new directory for the download
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/Report/ReportData.xlsx
+++ b/Group14-A2/src/main/java/Report/ReportData.xlsx
@@ -73,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -390,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -398,11 +399,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.17578125" collapsed="true" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.61328125" collapsed="true" customWidth="true" bestFit="true"/>
-    <col min="1" max="1" width="9.35546875" collapsed="true" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.61328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.8515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.35546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.61328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.17578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.61328125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.8515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -439,6 +440,23 @@
         <v>45408.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E3" t="n" s="2">
+        <v>45408.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>